<commit_message>
file and web.config update
update files and web.config
</commit_message>
<xml_diff>
--- a/HSNUAlumni.Web/contactsTemplate.xlsx
+++ b/HSNUAlumni.Web/contactsTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylee\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OnlineVS\HSNUAlumniProject\HSNUAlumniProject\HSNUAlumni.Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>ClassId</t>
   </si>
@@ -137,12 +137,6 @@
     <t xml:space="preserve">GENDER (性別) </t>
   </si>
   <si>
-    <t xml:space="preserve">男 - TRUE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">女 - FALSE </t>
-  </si>
-  <si>
     <t>Status (聯絡狀態) 限定在三類</t>
   </si>
   <si>
@@ -162,6 +156,18 @@
   </si>
   <si>
     <t xml:space="preserve">Birthday(生日) - 沒有預設 format 可設為任何一種字串 (With US system, it prefers MM/dd/yyyy) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">男 - M </t>
+  </si>
+  <si>
+    <t xml:space="preserve">女 - F </t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -499,7 +505,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -592,8 +598,8 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>47</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
@@ -639,8 +645,8 @@
       <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>48</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -696,19 +702,19 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,34 +722,34 @@
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>